<commit_message>
[Cloudstitch Services] Project publish veeyeetee/aaa
</commit_message>
<xml_diff>
--- a/API Spreadsheet.xlsx
+++ b/API Spreadsheet.xlsx
@@ -11,48 +11,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
-  <si>
-    <t>stripeStatus</t>
-  </si>
-  <si>
-    <t>stripeCustomerEmail</t>
-  </si>
-  <si>
-    <t>stripeCurrency</t>
-  </si>
-  <si>
-    <t>stripeAmount</t>
-  </si>
-  <si>
-    <t>stripeCreated</t>
-  </si>
-  <si>
-    <t>stripeDescription</t>
-  </si>
-  <si>
-    <t>stripeFailureMessage</t>
-  </si>
-  <si>
-    <t>succeeded</t>
-  </si>
-  <si>
-    <t>usd</t>
-  </si>
-  <si>
-    <t>A pretend book.</t>
-  </si>
-  <si>
-    <t>bertrand.keller@gmail.com</t>
-  </si>
-  <si>
-    <t>test@example.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>scanTime</t>
+  </si>
+  <si>
+    <t>scanTotal</t>
+  </si>
+  <si>
+    <t>scanSuccess</t>
+  </si>
+  <si>
+    <t>scanFail</t>
+  </si>
+  <si>
+    <t>scanTagScore</t>
+  </si>
+  <si>
+    <t>scanProduct</t>
+  </si>
+  <si>
+    <t>OG Kush</t>
+  </si>
+  <si>
+    <t>Blue Dream</t>
+  </si>
+  <si>
+    <t>Power OG</t>
+  </si>
+  <si>
+    <t>9# OG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm am/pm"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12.0"/>
@@ -95,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -106,6 +103,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -168,9 +168,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -189,73 +187,97 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" ht="15.75">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="4">
+        <v>0.3909722222222222</v>
+      </c>
+      <c r="B2" s="5">
+        <v>32.0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D5" si="1">B2-C2</f>
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75">
+      <c r="A3" s="4">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="B3" s="5">
+        <v>88.0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>87.0</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="4" ht="15.75">
+      <c r="A4" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="B4" s="5">
+        <v>124.0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>120.0</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
-        <v>100.0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1.498241007E9</v>
-      </c>
-      <c r="F2" s="4" t="s">
+    </row>
+    <row r="5" ht="15.75">
+      <c r="A5" s="4">
+        <v>0.3854166666666667</v>
+      </c>
+      <c r="B5" s="5">
+        <v>333.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>300.0</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="15.75">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4">
-        <v>100.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.500375581E9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1.506475224E9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="6"/>
-    </row>
     <row r="6">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8">
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[Cloudstitch Services] Project publish veeyeetee/cloudstitch-site
</commit_message>
<xml_diff>
--- a/API Spreadsheet.xlsx
+++ b/API Spreadsheet.xlsx
@@ -11,45 +11,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>scanTime</t>
-  </si>
-  <si>
-    <t>scanTotal</t>
-  </si>
-  <si>
-    <t>scanSuccess</t>
-  </si>
-  <si>
-    <t>scanFail</t>
-  </si>
-  <si>
-    <t>scanTagScore</t>
-  </si>
-  <si>
-    <t>scanProduct</t>
-  </si>
-  <si>
-    <t>OG Kush</t>
-  </si>
-  <si>
-    <t>Blue Dream</t>
-  </si>
-  <si>
-    <t>Power OG</t>
-  </si>
-  <si>
-    <t>9# OG</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+  <si>
+    <t>stripeStatus</t>
+  </si>
+  <si>
+    <t>stripeCustomerEmail</t>
+  </si>
+  <si>
+    <t>stripeCurrency</t>
+  </si>
+  <si>
+    <t>stripeAmount</t>
+  </si>
+  <si>
+    <t>stripeCreated</t>
+  </si>
+  <si>
+    <t>stripeDescription</t>
+  </si>
+  <si>
+    <t>stripeFailureMessage</t>
+  </si>
+  <si>
+    <t>succeeded</t>
+  </si>
+  <si>
+    <t>usd</t>
+  </si>
+  <si>
+    <t>A pretend book.</t>
+  </si>
+  <si>
+    <t>bertrand.keller@gmail.com</t>
+  </si>
+  <si>
+    <t>test@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="h:mm am/pm"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12.0"/>
@@ -92,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -103,9 +106,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -168,7 +168,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -187,97 +189,73 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" ht="15.75">
-      <c r="A2" s="4">
-        <v>0.3909722222222222</v>
-      </c>
-      <c r="B2" s="5">
-        <v>32.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>29.0</v>
-      </c>
-      <c r="D2" s="5">
-        <f t="shared" ref="D2:D5" si="1">B2-C2</f>
-        <v>3</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.498241007E9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="15.75">
-      <c r="A3" s="4">
-        <v>0.38958333333333334</v>
-      </c>
-      <c r="B3" s="5">
-        <v>88.0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>87.0</v>
-      </c>
-      <c r="D3" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.500375581E9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" ht="15.75">
-      <c r="A4" s="4">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="B4" s="5">
-        <v>124.0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>120.0</v>
-      </c>
-      <c r="D4" s="5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E4" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" ht="15.75">
-      <c r="A5" s="4">
-        <v>0.3854166666666667</v>
-      </c>
-      <c r="B5" s="5">
-        <v>333.0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>300.0</v>
-      </c>
-      <c r="D5" s="5">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="D4" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.506475224E9</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="C5" s="6"/>
+    </row>
     <row r="6">
-      <c r="C6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7">
-      <c r="C7" s="7"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8">
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>